<commit_message>
add new methods for excle
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t xml:space="preserve">Verify Login with valid data</t>
   </si>
@@ -46,10 +46,13 @@
     <t xml:space="preserve">Username</t>
   </si>
   <si>
+    <t xml:space="preserve">Data1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
     <t xml:space="preserve">test2@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,12 +162,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -184,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -235,27 +242,44 @@
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>12345</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
+      <c r="C7" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>456</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="2" t="n">
         <v>123</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>456</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>